<commit_message>
AU Actual and Results
</commit_message>
<xml_diff>
--- a/Admin/Suppliers/Manual testcases/Supplier Create New Supplier.xlsx
+++ b/Admin/Suppliers/Manual testcases/Supplier Create New Supplier.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zm-buyerautomation\Admin\Suppliers\Manual testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065BE09A-A7BE-4413-A647-AD3CFF34093A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE079568-4575-4560-8E8A-8C4B832DEC62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
   <si>
     <t>SL. No</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>Click on the Suppliers menu on the side navigation menubar</t>
-  </si>
-  <si>
-    <t>Application redirects to Suppliers screen+A2:E3</t>
   </si>
   <si>
     <t>Application get redirected to Suppliers screen</t>
@@ -260,6 +257,12 @@
       </rPr>
       <t xml:space="preserve">:Passive                                                                       Standard - billed anually dropdown                                                          CK - billed anually dropdown                                                                  Send subscription -related notification to....Enter email               </t>
     </r>
+  </si>
+  <si>
+    <t>Application redirects to Suppliers screen</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
@@ -360,7 +363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -383,6 +386,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -667,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,10 +734,13 @@
         <v>10</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>12</v>
+      <c r="G2" s="10" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -736,16 +751,19 @@
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>16</v>
+      <c r="G3" s="10" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -756,16 +774,19 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>19</v>
+      <c r="G4" s="11" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -776,19 +797,22 @@
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>21</v>
+      <c r="G5" s="10" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -796,16 +820,19 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="F6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>24</v>
+      <c r="G6" s="12" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -816,13 +843,19 @@
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -833,13 +866,19 @@
         <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>29</v>
+      <c r="F8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -850,13 +889,19 @@
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -867,13 +912,13 @@
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="9" t="s">
         <v>32</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>